<commit_message>
Ran parallel tests. Works great!
</commit_message>
<xml_diff>
--- a/Results/Stats/GA_P_4_N_20_results.xlsx
+++ b/Results/Stats/GA_P_4_N_20_results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\luker\source\repos\EC_P-Median\Results\Stats\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A718CC4-344D-4957-BE91-BCF2D8D12587}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3083FCC5-D1BE-42A5-B337-67611618AD42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,32 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="8">
+  <si>
+    <t>roulette</t>
+  </si>
+  <si>
+    <t>single_point</t>
+  </si>
+  <si>
+    <t>simple</t>
+  </si>
+  <si>
+    <t>double_point</t>
+  </si>
+  <si>
+    <t>hyper_heuristic</t>
+  </si>
+  <si>
+    <t>uniform</t>
+  </si>
+  <si>
+    <t>rank</t>
+  </si>
+  <si>
+    <t>touranment</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -336,14 +361,273 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:D18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="13.15625" customWidth="1"/>
+    <col min="2" max="2" width="14" customWidth="1"/>
+    <col min="3" max="3" width="15.9453125" customWidth="1"/>
+    <col min="4" max="4" width="17.05078125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1">
+        <v>5.3159552887507413</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2">
+        <v>5.3159552887507413</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3">
+        <v>5.3159552887507413</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D4">
+        <v>5.3159552887507413</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D5">
+        <v>5.3159552887507413</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D6">
+        <v>5.3159552887507413</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>3</v>
+      </c>
+      <c r="C7" t="s">
+        <v>2</v>
+      </c>
+      <c r="D7">
+        <v>5.3159552887507413</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A8" t="s">
+        <v>0</v>
+      </c>
+      <c r="B8" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8" t="s">
+        <v>4</v>
+      </c>
+      <c r="D8">
+        <v>5.3159552887507413</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A9" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9" t="s">
+        <v>1</v>
+      </c>
+      <c r="C9" t="s">
+        <v>4</v>
+      </c>
+      <c r="D9">
+        <v>5.3159552887507413</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A10" t="s">
+        <v>6</v>
+      </c>
+      <c r="B10" t="s">
+        <v>3</v>
+      </c>
+      <c r="C10" t="s">
+        <v>4</v>
+      </c>
+      <c r="D10">
+        <v>5.3159552887507413</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A11" t="s">
+        <v>7</v>
+      </c>
+      <c r="B11" t="s">
+        <v>1</v>
+      </c>
+      <c r="C11" t="s">
+        <v>2</v>
+      </c>
+      <c r="D11">
+        <v>5.3159552887507413</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A12" t="s">
+        <v>7</v>
+      </c>
+      <c r="B12" t="s">
+        <v>3</v>
+      </c>
+      <c r="C12" t="s">
+        <v>2</v>
+      </c>
+      <c r="D12">
+        <v>5.3159552887507413</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A13" t="s">
+        <v>6</v>
+      </c>
+      <c r="B13" t="s">
+        <v>5</v>
+      </c>
+      <c r="C13" t="s">
+        <v>2</v>
+      </c>
+      <c r="D13">
+        <v>5.3159552887507413</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A14" t="s">
+        <v>7</v>
+      </c>
+      <c r="B14" t="s">
+        <v>1</v>
+      </c>
+      <c r="C14" t="s">
+        <v>4</v>
+      </c>
+      <c r="D14">
+        <v>5.3159552887507413</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A15" t="s">
+        <v>6</v>
+      </c>
+      <c r="B15" t="s">
+        <v>5</v>
+      </c>
+      <c r="C15" t="s">
+        <v>4</v>
+      </c>
+      <c r="D15">
+        <v>5.3159552887507413</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A16" t="s">
+        <v>7</v>
+      </c>
+      <c r="B16" t="s">
+        <v>3</v>
+      </c>
+      <c r="C16" t="s">
+        <v>4</v>
+      </c>
+      <c r="D16">
+        <v>5.3159552887507413</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A17" t="s">
+        <v>7</v>
+      </c>
+      <c r="B17" t="s">
+        <v>5</v>
+      </c>
+      <c r="C17" t="s">
+        <v>2</v>
+      </c>
+      <c r="D17">
+        <v>5.3159552887507413</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A18" t="s">
+        <v>7</v>
+      </c>
+      <c r="B18" t="s">
+        <v>5</v>
+      </c>
+      <c r="C18" t="s">
+        <v>4</v>
+      </c>
+      <c r="D18">
+        <v>5.3159552887507413</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>